<commit_message>
Payment status of the Commissioners
</commit_message>
<xml_diff>
--- a/src/files/tempPDF/etatPaiemnt.xlsx
+++ b/src/files/tempPDF/etatPaiemnt.xlsx
@@ -11,21 +11,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Édité le : 18/02/2025 à 08:08:24
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t>Édité le : 26/02/2025 à 12:26:06
 Par : </t>
   </si>
   <si>
-    <t>État de paiement du commerçant : ALI JEMAA</t>
-  </si>
-  <si>
-    <t>Le : 17/02/2025</t>
+    <t>État de paiement des commerçants</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
+    <t>Client</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
@@ -44,7 +44,43 @@
     <t>Signataire</t>
   </si>
   <si>
+    <t>ALI JEMAA</t>
+  </si>
+  <si>
+    <t>Virement</t>
+  </si>
+  <si>
+    <t>Chèque</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>2025-02-18</t>
+  </si>
+  <si>
+    <t>ali</t>
+  </si>
+  <si>
+    <t>Espèce</t>
+  </si>
+  <si>
     <t>Remise</t>
+  </si>
+  <si>
+    <t>C1 C1</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>0123-01-01</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>FERHAT JEMAA</t>
   </si>
   <si>
     <t>Total</t>
@@ -189,21 +225,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="7" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="9" customWidth="1"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="7" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" customHeight="1">
+    <row r="1" spans="1:7" ht="30" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -212,8 +249,9 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" ht="40" customHeight="1">
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" ht="40" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -222,8 +260,9 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -232,67 +271,211 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="9">
+    <row r="6" spans="1:7">
+      <c r="A6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="9">
+        <v>45678</v>
+      </c>
+      <c r="C6" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="5"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="5"/>
+      <c r="B8" s="9">
+        <v>45677</v>
+      </c>
+      <c r="C8" s="10" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="5"/>
+      <c r="B9" s="9">
         <v>45705.69244213</v>
       </c>
-      <c r="B6" s="10" t="n">
+      <c r="C9" s="10" t="n">
         <v>25</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="13" t="n">
-        <v>25</v>
+      <c r="D9" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="9">
+        <v>45678</v>
+      </c>
+      <c r="C10" s="10" t="n">
+        <v>10000000</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="5"/>
+      <c r="B11" s="9">
+        <v>45688.95833333</v>
+      </c>
+      <c r="C11" s="10" t="n">
+        <v>45</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="9">
+        <v>45699</v>
+      </c>
+      <c r="C12" s="10" t="n">
+        <v>5000</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="12"/>
+      <c r="C13" s="13" t="n">
+        <v>10106920</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A6:A6"/>
-    <mergeCell ref="A7:A7"/>
+  <mergeCells count="13">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B8"/>
+    <mergeCell ref="B9:B9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B10"/>
+    <mergeCell ref="B11:B11"/>
+    <mergeCell ref="A12:A12"/>
+    <mergeCell ref="B12:B12"/>
+    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>